<commit_message>
included isSpecial column to item table in migration file
</commit_message>
<xml_diff>
--- a/backend/seed data.xlsx
+++ b/backend/seed data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Accelerate\BarExchange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Accelerate\DealingRoom\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA2F80E9-7E94-4063-8741-864025342D9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C1598B43-4420-4C50-9E3F-F553539AF554}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{EEBAA469-B6F4-4438-81E3-9D8DC8F7C6D9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="114">
   <si>
     <t>itemName</t>
   </si>
@@ -81,9 +81,6 @@
     <t>beer</t>
   </si>
   <si>
-    <t>Gwei Lo</t>
-  </si>
-  <si>
     <t>Mojito</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>Hennesey Paradis Imperial</t>
+  </si>
+  <si>
+    <t>Asa</t>
+  </si>
+  <si>
+    <t>Gweilo</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,7 @@
   <dimension ref="B1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +808,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -868,885 +871,888 @@
       <c r="F11" t="s">
         <v>17</v>
       </c>
+      <c r="I11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25">
         <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26">
         <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>100</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29">
         <v>100</v>
       </c>
       <c r="F29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30">
         <v>100</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31">
         <v>100</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>100</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>100</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <v>100</v>
       </c>
       <c r="F35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36">
         <v>100</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37">
         <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38">
         <v>100</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>100</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>100</v>
       </c>
       <c r="F40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41">
         <v>100</v>
       </c>
       <c r="F41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>100</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43">
         <v>100</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C44">
         <v>100</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <v>100</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46">
         <v>100</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C47">
         <v>100</v>
       </c>
       <c r="F47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C48">
         <v>100</v>
       </c>
       <c r="F48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49">
         <v>100</v>
       </c>
       <c r="F49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50">
         <v>100</v>
       </c>
       <c r="F50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C51">
         <v>100</v>
       </c>
       <c r="F51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52">
         <v>100</v>
       </c>
       <c r="F52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53">
         <v>100</v>
       </c>
       <c r="F53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54">
         <v>100</v>
       </c>
       <c r="F54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55">
         <v>100</v>
       </c>
       <c r="F55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56">
         <v>100</v>
       </c>
       <c r="F56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C57">
         <v>100</v>
       </c>
       <c r="F57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C58">
         <v>100</v>
       </c>
       <c r="F58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C59">
         <v>100</v>
       </c>
       <c r="F59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60">
         <v>100</v>
       </c>
       <c r="F60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61">
         <v>100</v>
       </c>
       <c r="F61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C62">
         <v>100</v>
       </c>
       <c r="F62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63">
         <v>100</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C64">
         <v>100</v>
       </c>
       <c r="F64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C65">
         <v>100</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66">
         <v>100</v>
       </c>
       <c r="F66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C67">
         <v>100</v>
       </c>
       <c r="F67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C68">
         <v>100</v>
       </c>
       <c r="F68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C69">
         <v>100</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C70">
         <v>100</v>
       </c>
       <c r="F70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C71">
         <v>100</v>
       </c>
       <c r="F71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C72">
         <v>100</v>
       </c>
       <c r="F72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C73">
         <v>100</v>
       </c>
       <c r="F73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C74">
         <v>100</v>
       </c>
       <c r="F74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C75">
         <v>100</v>
       </c>
       <c r="F75" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C76">
         <v>100</v>
       </c>
       <c r="F76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C77">
         <v>100</v>
       </c>
       <c r="F77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C78">
         <v>100</v>
       </c>
       <c r="F78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C79">
         <v>100</v>
       </c>
       <c r="F79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C80">
         <v>100</v>
       </c>
       <c r="F80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C81">
         <v>100</v>
       </c>
       <c r="F81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C82">
         <v>100</v>
       </c>
       <c r="F82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C83">
         <v>100</v>
       </c>
       <c r="F83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C84">
         <v>100</v>
       </c>
       <c r="F84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C85">
         <v>100</v>
       </c>
       <c r="F85" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C86">
         <v>100</v>
       </c>
       <c r="F86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C87">
         <v>100</v>
       </c>
       <c r="F87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C88">
         <v>100</v>
       </c>
       <c r="F88" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C89">
         <v>100</v>
       </c>
       <c r="F89" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C90">
         <v>100</v>
       </c>
       <c r="F90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C91">
         <v>100</v>
       </c>
       <c r="F91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorganized backend folders and installed proper dependecies
</commit_message>
<xml_diff>
--- a/backend/seed data.xlsx
+++ b/backend/seed data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Accelerate\DealingRoom\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{55D2F1C9-4AA7-43E2-B046-A8BA656B3758}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F1B19EFC-7435-4316-8A93-6D04358B7B8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{EEBAA469-B6F4-4438-81E3-9D8DC8F7C6D9}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,6 +509,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A342D5-895A-4836-B935-4060ED5EF9BC}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +842,7 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -899,8 +900,12 @@
       <c r="I2" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2">
+        <f>ROUNDUP((E2*1.05), 2)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -929,8 +934,12 @@
       <c r="I3" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <f>ROUNDUP((E3-($J$2-$E$2)/9),2)</f>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -959,8 +968,12 @@
       <c r="I4" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J11" si="1">ROUNDUP((E4-($J$2-$E$2)/9),2)</f>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -989,8 +1002,12 @@
       <c r="I5" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>79.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -1019,8 +1036,12 @@
       <c r="I6" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1049,8 +1070,12 @@
       <c r="I7" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1079,8 +1104,12 @@
       <c r="I8" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>79.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1109,8 +1138,12 @@
       <c r="I9" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1139,8 +1172,12 @@
       <c r="I10" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>59.669999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1169,8 +1206,20 @@
       <c r="I11" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>59.669999999999995</v>
+      </c>
+      <c r="K11" s="2">
+        <f>SUM(J2:J11)</f>
+        <v>640.03</v>
+      </c>
+      <c r="L11" s="4">
+        <f>SUM(E2:E11)</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1200,7 +1249,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1230,7 +1279,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1260,7 +1309,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1290,7 +1339,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1800,7 +1849,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1830,7 +1879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -1860,7 +1909,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -1890,7 +1939,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1920,7 +1969,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -1950,7 +1999,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -1980,7 +2029,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2010,7 +2059,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2040,7 +2089,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2070,7 +2119,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2099,8 +2148,12 @@
       <c r="I42" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1">
+        <f t="shared" ref="J42:J44" si="2">ROUNDUP((E42-($J$46-$E$46)/9),2)</f>
+        <v>78.89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2129,8 +2182,12 @@
       <c r="I43" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="1">
+        <f t="shared" si="2"/>
+        <v>78.89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2159,8 +2216,12 @@
       <c r="I44" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="1">
+        <f t="shared" si="2"/>
+        <v>98.89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -2189,8 +2250,12 @@
       <c r="I45" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="1">
+        <f>ROUNDUP((E45-($J$46-$E$46)/9),2)</f>
+        <v>118.89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -2219,8 +2284,20 @@
       <c r="I46" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="2">
+        <f>ROUNDUP((E46*1.05), 2)</f>
+        <v>210</v>
+      </c>
+      <c r="K46">
+        <f>SUM(J42:J46)</f>
+        <v>585.55999999999995</v>
+      </c>
+      <c r="L46" s="4">
+        <f>SUM(E42:E46)</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -2250,7 +2327,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2280,7 +2357,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2310,7 +2387,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2340,7 +2417,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2370,7 +2447,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2400,7 +2477,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2430,7 +2507,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -2460,7 +2537,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -2490,7 +2567,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -2520,7 +2597,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -2550,7 +2627,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>103</v>
       </c>
@@ -2580,7 +2657,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -2610,7 +2687,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>105</v>
       </c>
@@ -2640,7 +2717,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -2670,7 +2747,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -2699,8 +2776,12 @@
       <c r="I62" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="2">
+        <f>ROUNDUP((E62*1.05), 2)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>142</v>
       </c>
@@ -2729,8 +2810,12 @@
       <c r="I63" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="1">
+        <f>ROUNDUP((E63-($J$62-$E$62)/9),2)</f>
+        <v>99.56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>143</v>
       </c>
@@ -2759,8 +2844,12 @@
       <c r="I64" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="1">
+        <f t="shared" ref="J64:J66" si="3">ROUNDUP((E64-($J$62-$E$62)/9),2)</f>
+        <v>119.56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>144</v>
       </c>
@@ -2789,8 +2878,12 @@
       <c r="I65" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="1">
+        <f t="shared" si="3"/>
+        <v>199.56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>145</v>
       </c>
@@ -2819,8 +2912,20 @@
       <c r="I66" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="1">
+        <f t="shared" si="3"/>
+        <v>399.56</v>
+      </c>
+      <c r="K66">
+        <f>SUM(J62:J66)</f>
+        <v>902.24</v>
+      </c>
+      <c r="L66" s="4">
+        <f>SUM(E62:E66)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -2834,7 +2939,7 @@
         <v>10</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E91" si="1">D67*4</f>
+        <f t="shared" ref="E67:E91" si="4">D67*4</f>
         <v>40</v>
       </c>
       <c r="F67" t="s">
@@ -2850,7 +2955,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -2864,7 +2969,7 @@
         <v>10</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F68" t="s">
@@ -2880,7 +2985,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2894,7 +2999,7 @@
         <v>10</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F69" t="s">
@@ -2910,7 +3015,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>39</v>
       </c>
@@ -2924,7 +3029,7 @@
         <v>10</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F70" t="s">
@@ -2940,7 +3045,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>40</v>
       </c>
@@ -2954,7 +3059,7 @@
         <v>10</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F71" t="s">
@@ -2970,7 +3075,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -2984,7 +3089,7 @@
         <v>10</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F72" t="s">
@@ -3000,7 +3105,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -3014,7 +3119,7 @@
         <v>10</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F73" t="s">
@@ -3030,7 +3135,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -3044,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F74" t="s">
@@ -3060,7 +3165,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>44</v>
       </c>
@@ -3074,7 +3179,7 @@
         <v>10</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F75" t="s">
@@ -3090,7 +3195,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -3104,7 +3209,7 @@
         <v>10</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F76" t="s">
@@ -3120,7 +3225,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -3134,7 +3239,7 @@
         <v>15</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F77" t="s">
@@ -3150,7 +3255,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>58</v>
       </c>
@@ -3164,7 +3269,7 @@
         <v>15</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F78" t="s">
@@ -3180,7 +3285,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -3194,7 +3299,7 @@
         <v>15</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F79" t="s">
@@ -3210,7 +3315,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>49</v>
       </c>
@@ -3224,7 +3329,7 @@
         <v>15</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F80" t="s">
@@ -3254,7 +3359,7 @@
         <v>15</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F81" t="s">
@@ -3284,7 +3389,7 @@
         <v>30</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F82" t="s">
@@ -3314,7 +3419,7 @@
         <v>30</v>
       </c>
       <c r="E83" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F83" t="s">
@@ -3344,7 +3449,7 @@
         <v>30</v>
       </c>
       <c r="E84" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F84" t="s">
@@ -3374,7 +3479,7 @@
         <v>30</v>
       </c>
       <c r="E85" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F85" t="s">
@@ -3404,7 +3509,7 @@
         <v>30</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F86" t="s">
@@ -3434,7 +3539,7 @@
         <v>15</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F87" t="s">
@@ -3464,7 +3569,7 @@
         <v>15</v>
       </c>
       <c r="E88" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F88" t="s">
@@ -3494,7 +3599,7 @@
         <v>15</v>
       </c>
       <c r="E89" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F89" t="s">
@@ -3524,7 +3629,7 @@
         <v>15</v>
       </c>
       <c r="E90" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F90" t="s">
@@ -3554,7 +3659,7 @@
         <v>15</v>
       </c>
       <c r="E91" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F91" t="s">

</xml_diff>